<commit_message>
removendo as funcoes comentadas que usava multithead
</commit_message>
<xml_diff>
--- a/detailed_interactions_cards_done_list_marketplace.xlsx
+++ b/detailed_interactions_cards_done_list_marketplace.xlsx
@@ -20,7 +20,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -59,11 +62,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -21683,7 +21687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE132"/>
+  <dimension ref="A1:AF132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21845,6 +21849,11 @@
       <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>cardRole</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>movement_date</t>
         </is>
       </c>
     </row>
@@ -21931,7 +21940,7 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
@@ -21978,6 +21987,9 @@
         <v>0</v>
       </c>
       <c r="AE2" t="inlineStr"/>
+      <c r="AF2" s="2" t="n">
+        <v>45321.64441990741</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -22104,6 +22116,9 @@
         <v>0</v>
       </c>
       <c r="AE3" t="inlineStr"/>
+      <c r="AF3" s="2" t="n">
+        <v>45321.4846211574</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -22188,7 +22203,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -22235,6 +22250,9 @@
         <v>0</v>
       </c>
       <c r="AE4" t="inlineStr"/>
+      <c r="AF4" s="2" t="n">
+        <v>45320.86833048611</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -22357,6 +22375,9 @@
         <v>0</v>
       </c>
       <c r="AE5" t="inlineStr"/>
+      <c r="AF5" s="2" t="n">
+        <v>45320.74606923611</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -22448,7 +22469,7 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}, {'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}, {'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}]</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -22495,6 +22516,9 @@
         <v>0</v>
       </c>
       <c r="AE6" t="inlineStr"/>
+      <c r="AF6" s="2" t="n">
+        <v>45320.73730489583</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -22588,7 +22612,7 @@
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -22635,6 +22659,9 @@
         <v>0</v>
       </c>
       <c r="AE7" t="inlineStr"/>
+      <c r="AF7" s="2" t="n">
+        <v>45320.6677017824</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -22734,7 +22761,7 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -22781,6 +22808,9 @@
         <v>0</v>
       </c>
       <c r="AE8" t="inlineStr"/>
+      <c r="AF8" s="2" t="n">
+        <v>45317.66264984954</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -22879,7 +22909,7 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
@@ -22926,6 +22956,9 @@
         <v>0</v>
       </c>
       <c r="AE9" t="inlineStr"/>
+      <c r="AF9" s="2" t="n">
+        <v>45317.65143436343</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -23055,6 +23088,9 @@
         <v>0</v>
       </c>
       <c r="AE10" t="inlineStr"/>
+      <c r="AF10" s="2" t="n">
+        <v>45317.59274125</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -23177,6 +23213,9 @@
         <v>0</v>
       </c>
       <c r="AE11" t="inlineStr"/>
+      <c r="AF11" s="2" t="n">
+        <v>45315.95919740741</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -23311,6 +23350,9 @@
         <v>0</v>
       </c>
       <c r="AE12" t="inlineStr"/>
+      <c r="AF12" s="2" t="n">
+        <v>45314.85763059028</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -23403,7 +23445,7 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
@@ -23450,6 +23492,9 @@
         <v>0</v>
       </c>
       <c r="AE13" t="inlineStr"/>
+      <c r="AF13" s="2" t="n">
+        <v>45314.83411855324</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -23572,6 +23617,9 @@
         <v>0</v>
       </c>
       <c r="AE14" t="inlineStr"/>
+      <c r="AF14" s="2" t="n">
+        <v>45314.67953149306</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -23694,6 +23742,9 @@
         <v>0</v>
       </c>
       <c r="AE15" t="inlineStr"/>
+      <c r="AF15" s="2" t="n">
+        <v>45313.97050351852</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -23772,7 +23823,7 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
@@ -23819,6 +23870,9 @@
         <v>0</v>
       </c>
       <c r="AE16" t="inlineStr"/>
+      <c r="AF16" s="2" t="n">
+        <v>45310.75418130787</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -23941,6 +23995,9 @@
         <v>0</v>
       </c>
       <c r="AE17" t="inlineStr"/>
+      <c r="AF17" s="2" t="n">
+        <v>45310.75352620371</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -24025,7 +24082,7 @@
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
@@ -24072,6 +24129,9 @@
         <v>0</v>
       </c>
       <c r="AE18" t="inlineStr"/>
+      <c r="AF18" s="2" t="n">
+        <v>45310.67675300926</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -24168,7 +24228,7 @@
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
@@ -24215,6 +24275,9 @@
         <v>0</v>
       </c>
       <c r="AE19" t="inlineStr"/>
+      <c r="AF19" s="2" t="n">
+        <v>45310.58195571759</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -24309,7 +24372,7 @@
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
@@ -24356,6 +24419,9 @@
         <v>0</v>
       </c>
       <c r="AE20" t="inlineStr"/>
+      <c r="AF20" s="2" t="n">
+        <v>45310.57904549769</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -24433,7 +24499,7 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34de5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Spike / PoC', 'color': 'lime_light', 'uses': 78}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34de5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Spike / PoC', 'color': 'lime_light', 'uses': 78}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
@@ -24480,6 +24546,9 @@
         <v>0</v>
       </c>
       <c r="AE21" t="inlineStr"/>
+      <c r="AF21" s="2" t="n">
+        <v>45310.5128396875</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -24574,7 +24643,7 @@
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
@@ -24621,6 +24690,9 @@
         <v>0</v>
       </c>
       <c r="AE22" t="inlineStr"/>
+      <c r="AF22" s="2" t="n">
+        <v>45309.88025594907</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -24713,7 +24785,7 @@
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
@@ -24760,6 +24832,9 @@
         <v>0</v>
       </c>
       <c r="AE23" t="inlineStr"/>
+      <c r="AF23" s="2" t="n">
+        <v>45309.87965506945</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -24857,7 +24932,7 @@
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
@@ -24904,6 +24979,9 @@
         <v>0</v>
       </c>
       <c r="AE24" t="inlineStr"/>
+      <c r="AF24" s="2" t="n">
+        <v>45309.84264208333</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -24990,7 +25068,7 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}, {'id': '659d5c6046ba3d623b9a874f', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Bug external report', 'color': 'red_dark', 'uses': 1}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}, {'id': '659d5c6046ba3d623b9a874f', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Bug external report', 'color': 'red_dark', 'uses': 1}]</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
@@ -25037,6 +25115,9 @@
         <v>0</v>
       </c>
       <c r="AE25" t="inlineStr"/>
+      <c r="AF25" s="2" t="n">
+        <v>45309.77911354167</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -25135,7 +25216,7 @@
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
@@ -25182,6 +25263,9 @@
         <v>0</v>
       </c>
       <c r="AE26" t="inlineStr"/>
+      <c r="AF26" s="2" t="n">
+        <v>45309.6701758912</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -25304,6 +25388,9 @@
         <v>0</v>
       </c>
       <c r="AE27" t="inlineStr"/>
+      <c r="AF27" s="2" t="n">
+        <v>45309.65183231481</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -25426,6 +25513,9 @@
         <v>0</v>
       </c>
       <c r="AE28" t="inlineStr"/>
+      <c r="AF28" s="2" t="n">
+        <v>45309.65076390046</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -25548,6 +25638,9 @@
         <v>0</v>
       </c>
       <c r="AE29" t="inlineStr"/>
+      <c r="AF29" s="2" t="n">
+        <v>45309.64983065972</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -25670,6 +25763,9 @@
         <v>0</v>
       </c>
       <c r="AE30" t="inlineStr"/>
+      <c r="AF30" s="2" t="n">
+        <v>45309.64704370371</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -25792,6 +25888,9 @@
         <v>0</v>
       </c>
       <c r="AE31" t="inlineStr"/>
+      <c r="AF31" s="2" t="n">
+        <v>45309.64321545139</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -25869,7 +25968,7 @@
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>[{'id': '64f1e39bc8387ea7ef3c271e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Devops', 'color': 'green_light', 'uses': 2}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '64f1e39bc8387ea7ef3c271e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Devops', 'color': 'green_light', 'uses': 2}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T32" t="inlineStr">
@@ -25916,6 +26015,9 @@
         <v>0</v>
       </c>
       <c r="AE32" t="inlineStr"/>
+      <c r="AF32" s="2" t="n">
+        <v>45309.58682651621</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -26037,6 +26139,9 @@
         <v>0</v>
       </c>
       <c r="AE33" t="inlineStr"/>
+      <c r="AF33" s="2" t="n">
+        <v>45308.73196929398</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -26154,7 +26259,7 @@
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T34" t="inlineStr">
@@ -26201,6 +26306,9 @@
         <v>0</v>
       </c>
       <c r="AE34" t="inlineStr"/>
+      <c r="AF34" s="2" t="n">
+        <v>45307.82388806713</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -26292,7 +26400,7 @@
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
         </is>
       </c>
       <c r="T35" t="inlineStr">
@@ -26339,6 +26447,9 @@
         <v>0</v>
       </c>
       <c r="AE35" t="inlineStr"/>
+      <c r="AF35" s="2" t="n">
+        <v>45306.71879814815</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -26436,7 +26547,7 @@
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T36" t="inlineStr">
@@ -26483,6 +26594,9 @@
         <v>0</v>
       </c>
       <c r="AE36" t="inlineStr"/>
+      <c r="AF36" s="2" t="n">
+        <v>45306.68796200232</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -26578,7 +26692,7 @@
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '633e027dedd34201e1cc647c', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '📈 Data', 'color': 'purple_dark', 'uses': 104}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '633e027dedd34201e1cc647c', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '📈 Data', 'color': 'purple_dark', 'uses': 104}]</t>
         </is>
       </c>
       <c r="T37" t="inlineStr">
@@ -26625,6 +26739,9 @@
         <v>0</v>
       </c>
       <c r="AE37" t="inlineStr"/>
+      <c r="AF37" s="2" t="n">
+        <v>45303.50352185185</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -26697,7 +26814,7 @@
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T38" t="inlineStr">
@@ -26744,6 +26861,9 @@
         <v>0</v>
       </c>
       <c r="AE38" t="inlineStr"/>
+      <c r="AF38" s="2" t="n">
+        <v>45302.96849951389</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -26826,7 +26946,7 @@
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T39" t="inlineStr">
@@ -26873,6 +26993,9 @@
         <v>0</v>
       </c>
       <c r="AE39" t="inlineStr"/>
+      <c r="AF39" s="2" t="n">
+        <v>45302.96611523148</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -26958,7 +27081,7 @@
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}]</t>
         </is>
       </c>
       <c r="T40" t="inlineStr">
@@ -27005,6 +27128,9 @@
         <v>0</v>
       </c>
       <c r="AE40" t="inlineStr"/>
+      <c r="AF40" s="2" t="n">
+        <v>45302.96159962963</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -27079,7 +27205,7 @@
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T41" t="inlineStr">
@@ -27126,6 +27252,9 @@
         <v>0</v>
       </c>
       <c r="AE41" t="inlineStr"/>
+      <c r="AF41" s="2" t="n">
+        <v>45302.95861336806</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -27194,7 +27323,7 @@
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T42" t="inlineStr">
@@ -27241,6 +27370,9 @@
         <v>0</v>
       </c>
       <c r="AE42" t="inlineStr"/>
+      <c r="AF42" s="2" t="n">
+        <v>45302.9448496412</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -27325,7 +27457,7 @@
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
         </is>
       </c>
       <c r="T43" t="inlineStr">
@@ -27372,6 +27504,9 @@
         <v>0</v>
       </c>
       <c r="AE43" t="inlineStr"/>
+      <c r="AF43" s="2" t="n">
+        <v>45302.91460706019</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -27464,7 +27599,7 @@
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T44" t="inlineStr">
@@ -27511,6 +27646,9 @@
         <v>0</v>
       </c>
       <c r="AE44" t="inlineStr"/>
+      <c r="AF44" s="2" t="n">
+        <v>45302.89107320602</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -27606,7 +27744,7 @@
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T45" t="inlineStr">
@@ -27653,6 +27791,9 @@
         <v>0</v>
       </c>
       <c r="AE45" t="inlineStr"/>
+      <c r="AF45" s="2" t="n">
+        <v>45302.88931747685</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -27745,7 +27886,7 @@
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T46" t="inlineStr">
@@ -27792,6 +27933,9 @@
         <v>0</v>
       </c>
       <c r="AE46" t="inlineStr"/>
+      <c r="AF46" s="2" t="n">
+        <v>45302.84969537037</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -27885,7 +28029,7 @@
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T47" t="inlineStr">
@@ -27932,6 +28076,9 @@
         <v>0</v>
       </c>
       <c r="AE47" t="inlineStr"/>
+      <c r="AF47" s="2" t="n">
+        <v>45302.84855047454</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -28040,7 +28187,7 @@
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T48" t="inlineStr">
@@ -28087,6 +28234,9 @@
         <v>0</v>
       </c>
       <c r="AE48" t="inlineStr"/>
+      <c r="AF48" s="2" t="n">
+        <v>45302.82785723379</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -28179,7 +28329,7 @@
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
         </is>
       </c>
       <c r="T49" t="inlineStr">
@@ -28226,6 +28376,9 @@
         <v>0</v>
       </c>
       <c r="AE49" t="inlineStr"/>
+      <c r="AF49" s="2" t="n">
+        <v>45302.82566556713</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -28323,7 +28476,7 @@
       <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T50" t="inlineStr">
@@ -28370,6 +28523,9 @@
         <v>0</v>
       </c>
       <c r="AE50" t="inlineStr"/>
+      <c r="AF50" s="2" t="n">
+        <v>45302.8169397801</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -28446,7 +28602,7 @@
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T51" t="inlineStr">
@@ -28493,6 +28649,9 @@
         <v>0</v>
       </c>
       <c r="AE51" t="inlineStr"/>
+      <c r="AF51" s="2" t="n">
+        <v>45302.7340796412</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -28588,7 +28747,7 @@
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T52" t="inlineStr">
@@ -28635,6 +28794,9 @@
         <v>0</v>
       </c>
       <c r="AE52" t="inlineStr"/>
+      <c r="AF52" s="2" t="n">
+        <v>45301.95290150463</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -28716,7 +28878,7 @@
       <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T53" t="inlineStr">
@@ -28763,6 +28925,9 @@
         <v>0</v>
       </c>
       <c r="AE53" t="inlineStr"/>
+      <c r="AF53" s="2" t="n">
+        <v>45301.95218846065</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -28861,7 +29026,7 @@
       <c r="R54" t="inlineStr"/>
       <c r="S54" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T54" t="inlineStr">
@@ -28908,6 +29073,9 @@
         <v>0</v>
       </c>
       <c r="AE54" t="inlineStr"/>
+      <c r="AF54" s="2" t="n">
+        <v>45301.92891680555</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -29000,7 +29168,7 @@
       <c r="R55" t="inlineStr"/>
       <c r="S55" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T55" t="inlineStr">
@@ -29047,6 +29215,9 @@
         <v>0</v>
       </c>
       <c r="AE55" t="inlineStr"/>
+      <c r="AF55" s="2" t="n">
+        <v>45301.91510361111</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -29142,7 +29313,7 @@
       <c r="R56" t="inlineStr"/>
       <c r="S56" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T56" t="inlineStr">
@@ -29189,6 +29360,9 @@
         <v>0</v>
       </c>
       <c r="AE56" t="inlineStr"/>
+      <c r="AF56" s="2" t="n">
+        <v>45302.74915681713</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -29274,7 +29448,7 @@
       <c r="R57" t="inlineStr"/>
       <c r="S57" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
         </is>
       </c>
       <c r="T57" t="inlineStr">
@@ -29321,6 +29495,9 @@
         <v>0</v>
       </c>
       <c r="AE57" t="inlineStr"/>
+      <c r="AF57" s="2" t="n">
+        <v>45301.91164971065</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -29437,7 +29614,7 @@
       <c r="R58" t="inlineStr"/>
       <c r="S58" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T58" t="inlineStr">
@@ -29484,6 +29661,9 @@
         <v>0</v>
       </c>
       <c r="AE58" t="inlineStr"/>
+      <c r="AF58" s="2" t="n">
+        <v>45301.8640847338</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -29557,7 +29737,7 @@
       <c r="R59" t="inlineStr"/>
       <c r="S59" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}]</t>
         </is>
       </c>
       <c r="T59" t="inlineStr">
@@ -29604,6 +29784,9 @@
         <v>0</v>
       </c>
       <c r="AE59" t="inlineStr"/>
+      <c r="AF59" s="2" t="n">
+        <v>45301.72878667824</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -29694,7 +29877,7 @@
       <c r="R60" t="inlineStr"/>
       <c r="S60" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T60" t="inlineStr">
@@ -29741,6 +29924,9 @@
         <v>0</v>
       </c>
       <c r="AE60" t="inlineStr"/>
+      <c r="AF60" s="2" t="n">
+        <v>45301.72718171297</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -29833,7 +30019,7 @@
       <c r="R61" t="inlineStr"/>
       <c r="S61" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T61" t="inlineStr">
@@ -29880,6 +30066,9 @@
         <v>0</v>
       </c>
       <c r="AE61" t="inlineStr"/>
+      <c r="AF61" s="2" t="n">
+        <v>45301.71266525463</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -29972,7 +30161,7 @@
       <c r="R62" t="inlineStr"/>
       <c r="S62" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T62" t="inlineStr">
@@ -30019,6 +30208,9 @@
         <v>0</v>
       </c>
       <c r="AE62" t="inlineStr"/>
+      <c r="AF62" s="2" t="n">
+        <v>45301.70071818287</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -30118,7 +30310,7 @@
       <c r="R63" t="inlineStr"/>
       <c r="S63" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T63" t="inlineStr">
@@ -30165,6 +30357,9 @@
         <v>0</v>
       </c>
       <c r="AE63" t="inlineStr"/>
+      <c r="AF63" s="2" t="n">
+        <v>45301.6853140625</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -30261,7 +30456,7 @@
       <c r="R64" t="inlineStr"/>
       <c r="S64" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '6511addb155e1a5481981d69', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Android', 'color': 'green_dark', 'uses': 15}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '6511addb155e1a5481981d69', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Android', 'color': 'green_dark', 'uses': 15}]</t>
         </is>
       </c>
       <c r="T64" t="inlineStr">
@@ -30308,6 +30503,9 @@
         <v>0</v>
       </c>
       <c r="AE64" t="inlineStr"/>
+      <c r="AF64" s="2" t="n">
+        <v>45301.60337752315</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -30394,7 +30592,7 @@
       <c r="R65" t="inlineStr"/>
       <c r="S65" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
         </is>
       </c>
       <c r="T65" t="inlineStr">
@@ -30441,6 +30639,9 @@
         <v>0</v>
       </c>
       <c r="AE65" t="inlineStr"/>
+      <c r="AF65" s="2" t="n">
+        <v>45300.98007916666</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -30544,7 +30745,7 @@
       <c r="R66" t="inlineStr"/>
       <c r="S66" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '633e027dedd34201e1cc647c', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '📈 Data', 'color': 'purple_dark', 'uses': 104}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '633e027dedd34201e1cc647c', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '📈 Data', 'color': 'purple_dark', 'uses': 104}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T66" t="inlineStr">
@@ -30591,6 +30792,9 @@
         <v>0</v>
       </c>
       <c r="AE66" t="inlineStr"/>
+      <c r="AF66" s="2" t="n">
+        <v>45296.79376248843</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -30716,6 +30920,9 @@
         <v>0</v>
       </c>
       <c r="AE67" t="inlineStr"/>
+      <c r="AF67" s="2" t="n">
+        <v>45296.57727751158</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -30812,7 +31019,7 @@
       <c r="R68" t="inlineStr"/>
       <c r="S68" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T68" t="inlineStr">
@@ -30859,6 +31066,9 @@
         <v>0</v>
       </c>
       <c r="AE68" t="inlineStr"/>
+      <c r="AF68" s="2" t="n">
+        <v>45294.94193791666</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -30982,6 +31192,9 @@
         <v>0</v>
       </c>
       <c r="AE69" t="inlineStr"/>
+      <c r="AF69" s="2" t="n">
+        <v>45294.94122461806</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -31070,7 +31283,7 @@
       <c r="R70" t="inlineStr"/>
       <c r="S70" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T70" t="inlineStr">
@@ -31117,6 +31330,9 @@
         <v>0</v>
       </c>
       <c r="AE70" t="inlineStr"/>
+      <c r="AF70" s="2" t="n">
+        <v>45294.86376837963</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -31246,6 +31462,9 @@
         <v>0</v>
       </c>
       <c r="AE71" t="inlineStr"/>
+      <c r="AF71" s="2" t="n">
+        <v>45294.85913269676</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -31376,6 +31595,9 @@
         <v>0</v>
       </c>
       <c r="AE72" t="inlineStr"/>
+      <c r="AF72" s="2" t="n">
+        <v>45294.81978753473</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -31506,6 +31728,9 @@
         <v>0</v>
       </c>
       <c r="AE73" t="inlineStr"/>
+      <c r="AF73" s="2" t="n">
+        <v>45294.81969760417</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -31636,6 +31861,9 @@
         <v>0</v>
       </c>
       <c r="AE74" t="inlineStr"/>
+      <c r="AF74" s="2" t="n">
+        <v>45294.81958255787</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -31758,6 +31986,9 @@
         <v>0</v>
       </c>
       <c r="AE75" t="inlineStr"/>
+      <c r="AF75" s="2" t="n">
+        <v>45288.72397538194</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -31860,7 +32091,7 @@
       <c r="R76" t="inlineStr"/>
       <c r="S76" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T76" t="inlineStr">
@@ -31907,6 +32138,9 @@
         <v>0</v>
       </c>
       <c r="AE76" t="inlineStr"/>
+      <c r="AF76" s="2" t="n">
+        <v>45282.58166978009</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -31999,7 +32233,7 @@
       <c r="R77" t="inlineStr"/>
       <c r="S77" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
         </is>
       </c>
       <c r="T77" t="inlineStr">
@@ -32046,6 +32280,9 @@
         <v>0</v>
       </c>
       <c r="AE77" t="inlineStr"/>
+      <c r="AF77" s="2" t="n">
+        <v>45282.57716027777</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -32141,7 +32378,7 @@
       <c r="R78" t="inlineStr"/>
       <c r="S78" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T78" t="inlineStr">
@@ -32188,6 +32425,9 @@
         <v>0</v>
       </c>
       <c r="AE78" t="inlineStr"/>
+      <c r="AF78" s="2" t="n">
+        <v>45281.94473803241</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -32283,7 +32523,7 @@
       <c r="R79" t="inlineStr"/>
       <c r="S79" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T79" t="inlineStr">
@@ -32330,6 +32570,9 @@
         <v>0</v>
       </c>
       <c r="AE79" t="inlineStr"/>
+      <c r="AF79" s="2" t="n">
+        <v>45281.86092715277</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -32445,7 +32688,7 @@
       <c r="R80" t="inlineStr"/>
       <c r="S80" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T80" t="inlineStr">
@@ -32492,6 +32735,9 @@
         <v>0</v>
       </c>
       <c r="AE80" t="inlineStr"/>
+      <c r="AF80" s="2" t="n">
+        <v>45281.77926972222</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -32586,7 +32832,7 @@
       <c r="R81" t="inlineStr"/>
       <c r="S81" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T81" t="inlineStr">
@@ -32633,6 +32879,9 @@
         <v>0</v>
       </c>
       <c r="AE81" t="inlineStr"/>
+      <c r="AF81" s="2" t="n">
+        <v>45281.77924885417</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -32733,7 +32982,7 @@
       <c r="R82" t="inlineStr"/>
       <c r="S82" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T82" t="inlineStr">
@@ -32780,6 +33029,9 @@
         <v>0</v>
       </c>
       <c r="AE82" t="inlineStr"/>
+      <c r="AF82" s="2" t="n">
+        <v>45281.64254180556</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -32898,7 +33150,7 @@
       <c r="R83" t="inlineStr"/>
       <c r="S83" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T83" t="inlineStr">
@@ -32945,6 +33197,9 @@
         <v>0</v>
       </c>
       <c r="AE83" t="inlineStr"/>
+      <c r="AF83" s="2" t="n">
+        <v>45281.43172827546</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -33041,7 +33296,7 @@
       <c r="R84" t="inlineStr"/>
       <c r="S84" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T84" t="inlineStr">
@@ -33088,6 +33343,9 @@
         <v>0</v>
       </c>
       <c r="AE84" t="inlineStr"/>
+      <c r="AF84" s="2" t="n">
+        <v>45281.4215430324</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -33180,7 +33438,7 @@
       <c r="R85" t="inlineStr"/>
       <c r="S85" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T85" t="inlineStr">
@@ -33227,6 +33485,9 @@
         <v>0</v>
       </c>
       <c r="AE85" t="inlineStr"/>
+      <c r="AF85" s="2" t="n">
+        <v>45281.41371859954</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -33314,7 +33575,7 @@
       <c r="R86" t="inlineStr"/>
       <c r="S86" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T86" t="inlineStr">
@@ -33361,6 +33622,9 @@
         <v>0</v>
       </c>
       <c r="AE86" t="inlineStr"/>
+      <c r="AF86" s="2" t="n">
+        <v>45280.7736556713</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -33457,7 +33721,7 @@
       <c r="R87" t="inlineStr"/>
       <c r="S87" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T87" t="inlineStr">
@@ -33504,6 +33768,9 @@
         <v>0</v>
       </c>
       <c r="AE87" t="inlineStr"/>
+      <c r="AF87" s="2" t="n">
+        <v>45280.77282775463</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -33598,7 +33865,7 @@
       <c r="R88" t="inlineStr"/>
       <c r="S88" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T88" t="inlineStr">
@@ -33645,6 +33912,9 @@
         <v>0</v>
       </c>
       <c r="AE88" t="inlineStr"/>
+      <c r="AF88" s="2" t="n">
+        <v>45280.72932037037</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -33737,7 +34007,7 @@
       <c r="R89" t="inlineStr"/>
       <c r="S89" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T89" t="inlineStr">
@@ -33784,6 +34054,9 @@
         <v>0</v>
       </c>
       <c r="AE89" t="inlineStr"/>
+      <c r="AF89" s="2" t="n">
+        <v>45280.7215578125</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -33860,7 +34133,7 @@
       </c>
       <c r="S90" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}, {'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T90" t="inlineStr">
@@ -33907,6 +34180,9 @@
         <v>0</v>
       </c>
       <c r="AE90" t="inlineStr"/>
+      <c r="AF90" s="2" t="n">
+        <v>45280.69797907407</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -34008,7 +34284,7 @@
       <c r="R91" t="inlineStr"/>
       <c r="S91" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T91" t="inlineStr">
@@ -34055,6 +34331,9 @@
         <v>0</v>
       </c>
       <c r="AE91" t="inlineStr"/>
+      <c r="AF91" s="2" t="n">
+        <v>45279.9587033912</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -34141,7 +34420,7 @@
       <c r="R92" t="inlineStr"/>
       <c r="S92" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
         </is>
       </c>
       <c r="T92" t="inlineStr">
@@ -34188,6 +34467,9 @@
         <v>0</v>
       </c>
       <c r="AE92" t="inlineStr"/>
+      <c r="AF92" s="2" t="n">
+        <v>45279.84811211805</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -34272,7 +34554,7 @@
       <c r="R93" t="inlineStr"/>
       <c r="S93" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}, {'id': '64ac7e1ce382db5540cf8348', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'iOS', 'color': 'black_light', 'uses': 19}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}, {'id': '64ac7e1ce382db5540cf8348', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'iOS', 'color': 'black_light', 'uses': 19}]</t>
         </is>
       </c>
       <c r="T93" t="inlineStr">
@@ -34319,6 +34601,9 @@
         <v>0</v>
       </c>
       <c r="AE93" t="inlineStr"/>
+      <c r="AF93" s="2" t="n">
+        <v>45278.91231490741</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -34403,7 +34688,7 @@
       <c r="R94" t="inlineStr"/>
       <c r="S94" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}, {'id': '6511addb155e1a5481981d69', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Android', 'color': 'green_dark', 'uses': 15}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}, {'id': '6511addb155e1a5481981d69', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Android', 'color': 'green_dark', 'uses': 15}]</t>
         </is>
       </c>
       <c r="T94" t="inlineStr">
@@ -34450,6 +34735,9 @@
         <v>0</v>
       </c>
       <c r="AE94" t="inlineStr"/>
+      <c r="AF94" s="2" t="n">
+        <v>45278.91229980324</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -34545,7 +34833,7 @@
       <c r="R95" t="inlineStr"/>
       <c r="S95" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T95" t="inlineStr">
@@ -34592,6 +34880,9 @@
         <v>0</v>
       </c>
       <c r="AE95" t="inlineStr"/>
+      <c r="AF95" s="2" t="n">
+        <v>45278.88792607639</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -34686,7 +34977,7 @@
       <c r="R96" t="inlineStr"/>
       <c r="S96" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T96" t="inlineStr">
@@ -34733,6 +35024,9 @@
         <v>0</v>
       </c>
       <c r="AE96" t="inlineStr"/>
+      <c r="AF96" s="2" t="n">
+        <v>45274.67148517361</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -34820,7 +35114,7 @@
       <c r="R97" t="inlineStr"/>
       <c r="S97" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T97" t="inlineStr">
@@ -34867,6 +35161,9 @@
         <v>0</v>
       </c>
       <c r="AE97" t="inlineStr"/>
+      <c r="AF97" s="2" t="n">
+        <v>45273.83550787037</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -34958,7 +35255,7 @@
       <c r="R98" t="inlineStr"/>
       <c r="S98" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T98" t="inlineStr">
@@ -35005,6 +35302,9 @@
         <v>0</v>
       </c>
       <c r="AE98" t="inlineStr"/>
+      <c r="AF98" s="2" t="n">
+        <v>45273.50947658565</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -35092,7 +35392,7 @@
       <c r="R99" t="inlineStr"/>
       <c r="S99" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T99" t="inlineStr">
@@ -35139,6 +35439,9 @@
         <v>0</v>
       </c>
       <c r="AE99" t="inlineStr"/>
+      <c r="AF99" s="2" t="n">
+        <v>45272.8678574537</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -35233,7 +35536,7 @@
       <c r="R100" t="inlineStr"/>
       <c r="S100" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T100" t="inlineStr">
@@ -35280,6 +35583,9 @@
         <v>0</v>
       </c>
       <c r="AE100" t="inlineStr"/>
+      <c r="AF100" s="2" t="n">
+        <v>45272.66151157407</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -35374,7 +35680,7 @@
       <c r="R101" t="inlineStr"/>
       <c r="S101" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T101" t="inlineStr">
@@ -35421,6 +35727,9 @@
         <v>0</v>
       </c>
       <c r="AE101" t="inlineStr"/>
+      <c r="AF101" s="2" t="n">
+        <v>45272.58665163194</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -35530,7 +35839,7 @@
       <c r="R102" t="inlineStr"/>
       <c r="S102" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T102" t="inlineStr">
@@ -35577,6 +35886,9 @@
         <v>0</v>
       </c>
       <c r="AE102" t="inlineStr"/>
+      <c r="AF102" s="2" t="n">
+        <v>45271.7538206713</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -35671,7 +35983,7 @@
       <c r="R103" t="inlineStr"/>
       <c r="S103" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '6511addb155e1a5481981d69', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Android', 'color': 'green_dark', 'uses': 15}, {'id': '64ac7e1ce382db5540cf8348', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'iOS', 'color': 'black_light', 'uses': 19}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '6511addb155e1a5481981d69', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Android', 'color': 'green_dark', 'uses': 15}, {'id': '64ac7e1ce382db5540cf8348', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'iOS', 'color': 'black_light', 'uses': 19}]</t>
         </is>
       </c>
       <c r="T103" t="inlineStr">
@@ -35718,6 +36030,9 @@
         <v>0</v>
       </c>
       <c r="AE103" t="inlineStr"/>
+      <c r="AF103" s="2" t="n">
+        <v>45271.72398444444</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -35812,7 +36127,7 @@
       <c r="R104" t="inlineStr"/>
       <c r="S104" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T104" t="inlineStr">
@@ -35859,6 +36174,9 @@
         <v>0</v>
       </c>
       <c r="AE104" t="inlineStr"/>
+      <c r="AF104" s="2" t="n">
+        <v>45271.72200959491</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -35966,7 +36284,7 @@
       <c r="R105" t="inlineStr"/>
       <c r="S105" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T105" t="inlineStr">
@@ -36013,6 +36331,9 @@
         <v>0</v>
       </c>
       <c r="AE105" t="inlineStr"/>
+      <c r="AF105" s="2" t="n">
+        <v>45271.71038612269</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -36148,6 +36469,9 @@
         <v>0</v>
       </c>
       <c r="AE106" t="inlineStr"/>
+      <c r="AF106" s="2" t="n">
+        <v>45271.71029019676</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -36238,7 +36562,7 @@
       <c r="R107" t="inlineStr"/>
       <c r="S107" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T107" t="inlineStr">
@@ -36285,6 +36609,9 @@
         <v>0</v>
       </c>
       <c r="AE107" t="inlineStr"/>
+      <c r="AF107" s="2" t="n">
+        <v>45271.71018223379</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -36379,7 +36706,7 @@
       <c r="R108" t="inlineStr"/>
       <c r="S108" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}]</t>
         </is>
       </c>
       <c r="T108" t="inlineStr">
@@ -36426,6 +36753,9 @@
         <v>0</v>
       </c>
       <c r="AE108" t="inlineStr"/>
+      <c r="AF108" s="2" t="n">
+        <v>45271.67947991898</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -36516,7 +36846,7 @@
       <c r="R109" t="inlineStr"/>
       <c r="S109" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}]</t>
         </is>
       </c>
       <c r="T109" t="inlineStr">
@@ -36563,6 +36893,9 @@
         <v>0</v>
       </c>
       <c r="AE109" t="inlineStr"/>
+      <c r="AF109" s="2" t="n">
+        <v>45271.61266383102</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -36639,7 +36972,7 @@
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T110" t="inlineStr">
@@ -36686,6 +37019,9 @@
         <v>0</v>
       </c>
       <c r="AE110" t="inlineStr"/>
+      <c r="AF110" s="2" t="n">
+        <v>45267.98361020834</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -36782,7 +37118,7 @@
       <c r="R111" t="inlineStr"/>
       <c r="S111" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T111" t="inlineStr">
@@ -36829,6 +37165,9 @@
         <v>0</v>
       </c>
       <c r="AE111" t="inlineStr"/>
+      <c r="AF111" s="2" t="n">
+        <v>45267.94140542824</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -36922,7 +37261,7 @@
       <c r="R112" t="inlineStr"/>
       <c r="S112" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T112" t="inlineStr">
@@ -36969,6 +37308,9 @@
         <v>0</v>
       </c>
       <c r="AE112" t="inlineStr"/>
+      <c r="AF112" s="2" t="n">
+        <v>45267.91566591436</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -37070,7 +37412,7 @@
       <c r="R113" t="inlineStr"/>
       <c r="S113" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}]</t>
         </is>
       </c>
       <c r="T113" t="inlineStr">
@@ -37117,6 +37459,9 @@
         <v>0</v>
       </c>
       <c r="AE113" t="inlineStr"/>
+      <c r="AF113" s="2" t="n">
+        <v>45267.91441982639</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -37222,7 +37567,7 @@
       <c r="R114" t="inlineStr"/>
       <c r="S114" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T114" t="inlineStr">
@@ -37269,6 +37614,9 @@
         <v>0</v>
       </c>
       <c r="AE114" t="inlineStr"/>
+      <c r="AF114" s="2" t="n">
+        <v>45267.91422902778</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -37384,7 +37732,7 @@
       <c r="R115" t="inlineStr"/>
       <c r="S115" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T115" t="inlineStr">
@@ -37431,6 +37779,9 @@
         <v>0</v>
       </c>
       <c r="AE115" t="inlineStr"/>
+      <c r="AF115" s="2" t="n">
+        <v>45267.91249532408</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -37519,7 +37870,7 @@
       <c r="R116" t="inlineStr"/>
       <c r="S116" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}]</t>
         </is>
       </c>
       <c r="T116" t="inlineStr">
@@ -37566,6 +37917,9 @@
         <v>0</v>
       </c>
       <c r="AE116" t="inlineStr"/>
+      <c r="AF116" s="2" t="n">
+        <v>45267.91070800926</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -37658,7 +38012,7 @@
       <c r="R117" t="inlineStr"/>
       <c r="S117" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T117" t="inlineStr">
@@ -37705,6 +38059,9 @@
         <v>0</v>
       </c>
       <c r="AE117" t="inlineStr"/>
+      <c r="AF117" s="2" t="n">
+        <v>45267.89615033565</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -37799,7 +38156,7 @@
       <c r="R118" t="inlineStr"/>
       <c r="S118" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T118" t="inlineStr">
@@ -37846,6 +38203,9 @@
         <v>0</v>
       </c>
       <c r="AE118" t="inlineStr"/>
+      <c r="AF118" s="2" t="n">
+        <v>45267.88008541667</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -37940,7 +38300,7 @@
       <c r="R119" t="inlineStr"/>
       <c r="S119" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T119" t="inlineStr">
@@ -37987,6 +38347,9 @@
         <v>0</v>
       </c>
       <c r="AE119" t="inlineStr"/>
+      <c r="AF119" s="2" t="n">
+        <v>45267.87417387732</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -38081,7 +38444,7 @@
       <c r="R120" t="inlineStr"/>
       <c r="S120" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T120" t="inlineStr">
@@ -38128,6 +38491,9 @@
         <v>0</v>
       </c>
       <c r="AE120" t="inlineStr"/>
+      <c r="AF120" s="2" t="n">
+        <v>45267.87207349537</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -38218,7 +38584,7 @@
       <c r="R121" t="inlineStr"/>
       <c r="S121" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
         </is>
       </c>
       <c r="T121" t="inlineStr">
@@ -38265,6 +38631,9 @@
         <v>0</v>
       </c>
       <c r="AE121" t="inlineStr"/>
+      <c r="AF121" s="2" t="n">
+        <v>45267.75843868055</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -38337,7 +38706,7 @@
       </c>
       <c r="S122" t="inlineStr">
         <is>
-          <t>[{'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}, {'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}]</t>
+          <t>[{'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}]</t>
         </is>
       </c>
       <c r="T122" t="inlineStr">
@@ -38384,6 +38753,9 @@
         <v>0</v>
       </c>
       <c r="AE122" t="inlineStr"/>
+      <c r="AF122" s="2" t="n">
+        <v>45266.91523304398</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -38460,7 +38832,7 @@
       </c>
       <c r="S123" t="inlineStr">
         <is>
-          <t>[{'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}, {'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}]</t>
+          <t>[{'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}]</t>
         </is>
       </c>
       <c r="T123" t="inlineStr">
@@ -38507,6 +38879,9 @@
         <v>0</v>
       </c>
       <c r="AE123" t="inlineStr"/>
+      <c r="AF123" s="2" t="n">
+        <v>45266.91514569445</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -38585,7 +38960,7 @@
       </c>
       <c r="S124" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 233}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T124" t="inlineStr">
@@ -38632,6 +39007,9 @@
         <v>0</v>
       </c>
       <c r="AE124" t="inlineStr"/>
+      <c r="AF124" s="2" t="n">
+        <v>45265.59286556713</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -38737,7 +39115,7 @@
       <c r="R125" t="inlineStr"/>
       <c r="S125" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 369}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T125" t="inlineStr">
@@ -38784,6 +39162,9 @@
         <v>0</v>
       </c>
       <c r="AE125" t="inlineStr"/>
+      <c r="AF125" s="2" t="n">
+        <v>45264.91138417824</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -38879,7 +39260,7 @@
       <c r="R126" t="inlineStr"/>
       <c r="S126" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}, {'id': '633e027dedd34201e1cc647c', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '📈 Data', 'color': 'purple_dark', 'uses': 104}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '633e027dedd34201e1cc647c', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '📈 Data', 'color': 'purple_dark', 'uses': 104}]</t>
         </is>
       </c>
       <c r="T126" t="inlineStr">
@@ -38926,6 +39307,9 @@
         <v>0</v>
       </c>
       <c r="AE126" t="inlineStr"/>
+      <c r="AF126" s="2" t="n">
+        <v>45264.90938443287</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -39024,7 +39408,7 @@
       <c r="R127" t="inlineStr"/>
       <c r="S127" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T127" t="inlineStr">
@@ -39071,6 +39455,9 @@
         <v>0</v>
       </c>
       <c r="AE127" t="inlineStr"/>
+      <c r="AF127" s="2" t="n">
+        <v>45264.90421420139</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -39156,7 +39543,7 @@
       </c>
       <c r="S128" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 196}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
         </is>
       </c>
       <c r="T128" t="inlineStr">
@@ -39203,6 +39590,9 @@
         <v>0</v>
       </c>
       <c r="AE128" t="inlineStr"/>
+      <c r="AF128" s="2" t="n">
+        <v>45264.90345635416</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -39332,6 +39722,9 @@
         <v>0</v>
       </c>
       <c r="AE129" t="inlineStr"/>
+      <c r="AF129" s="2" t="n">
+        <v>45264.88809135417</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -39424,7 +39817,7 @@
       <c r="R130" t="inlineStr"/>
       <c r="S130" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 321}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}]</t>
         </is>
       </c>
       <c r="T130" t="inlineStr">
@@ -39471,6 +39864,9 @@
         <v>0</v>
       </c>
       <c r="AE130" t="inlineStr"/>
+      <c r="AF130" s="2" t="n">
+        <v>45264.68942390046</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -39543,7 +39939,7 @@
       <c r="R131" t="inlineStr"/>
       <c r="S131" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 86}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}]</t>
         </is>
       </c>
       <c r="T131" t="inlineStr">
@@ -39590,6 +39986,9 @@
         <v>0</v>
       </c>
       <c r="AE131" t="inlineStr"/>
+      <c r="AF131" s="2" t="n">
+        <v>45264.68928572917</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -39714,6 +40113,9 @@
         <v>0</v>
       </c>
       <c r="AE132" t="inlineStr"/>
+      <c r="AF132" s="2" t="n">
+        <v>45261.62664386574</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add os projetos de langchain
</commit_message>
<xml_diff>
--- a/detailed_interactions_cards_done_list_marketplace.xlsx
+++ b/detailed_interactions_cards_done_list_marketplace.xlsx
@@ -22469,7 +22469,7 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}, {'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}, {'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}]</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -22761,7 +22761,7 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -23445,7 +23445,7 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
@@ -23823,7 +23823,7 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '6334974f95f46800f751eb21', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🧪️ QA', 'color': 'lime', 'uses': 127}]</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
@@ -24228,7 +24228,7 @@
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
@@ -24499,7 +24499,7 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34de5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Spike / PoC', 'color': 'lime_light', 'uses': 78}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34de5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Spike / PoC', 'color': 'lime_light', 'uses': 78}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
@@ -25968,7 +25968,7 @@
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>[{'id': '64f1e39bc8387ea7ef3c271e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Devops', 'color': 'green_light', 'uses': 2}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '64f1e39bc8387ea7ef3c271e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Devops', 'color': 'green_light', 'uses': 2}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T32" t="inlineStr">
@@ -26259,7 +26259,7 @@
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T34" t="inlineStr">
@@ -26814,7 +26814,7 @@
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T38" t="inlineStr">
@@ -26946,7 +26946,7 @@
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T39" t="inlineStr">
@@ -27081,7 +27081,7 @@
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}]</t>
         </is>
       </c>
       <c r="T40" t="inlineStr">
@@ -27205,7 +27205,7 @@
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T41" t="inlineStr">
@@ -27323,7 +27323,7 @@
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T42" t="inlineStr">
@@ -28602,7 +28602,7 @@
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T51" t="inlineStr">
@@ -28878,7 +28878,7 @@
       <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T53" t="inlineStr">
@@ -29026,7 +29026,7 @@
       <c r="R54" t="inlineStr"/>
       <c r="S54" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T54" t="inlineStr">
@@ -29737,7 +29737,7 @@
       <c r="R59" t="inlineStr"/>
       <c r="S59" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}]</t>
         </is>
       </c>
       <c r="T59" t="inlineStr">
@@ -29877,7 +29877,7 @@
       <c r="R60" t="inlineStr"/>
       <c r="S60" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T60" t="inlineStr">
@@ -30310,7 +30310,7 @@
       <c r="R63" t="inlineStr"/>
       <c r="S63" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T63" t="inlineStr">
@@ -31019,7 +31019,7 @@
       <c r="R68" t="inlineStr"/>
       <c r="S68" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T68" t="inlineStr">
@@ -31283,7 +31283,7 @@
       <c r="R70" t="inlineStr"/>
       <c r="S70" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T70" t="inlineStr">
@@ -32378,7 +32378,7 @@
       <c r="R78" t="inlineStr"/>
       <c r="S78" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T78" t="inlineStr">
@@ -32523,7 +32523,7 @@
       <c r="R79" t="inlineStr"/>
       <c r="S79" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T79" t="inlineStr">
@@ -32688,7 +32688,7 @@
       <c r="R80" t="inlineStr"/>
       <c r="S80" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T80" t="inlineStr">
@@ -32982,7 +32982,7 @@
       <c r="R82" t="inlineStr"/>
       <c r="S82" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T82" t="inlineStr">
@@ -33150,7 +33150,7 @@
       <c r="R83" t="inlineStr"/>
       <c r="S83" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T83" t="inlineStr">
@@ -33438,7 +33438,7 @@
       <c r="R85" t="inlineStr"/>
       <c r="S85" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T85" t="inlineStr">
@@ -34133,7 +34133,7 @@
       </c>
       <c r="S90" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}, {'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}]</t>
         </is>
       </c>
       <c r="T90" t="inlineStr">
@@ -34284,7 +34284,7 @@
       <c r="R91" t="inlineStr"/>
       <c r="S91" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T91" t="inlineStr">
@@ -34833,7 +34833,7 @@
       <c r="R95" t="inlineStr"/>
       <c r="S95" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T95" t="inlineStr">
@@ -35114,7 +35114,7 @@
       <c r="R97" t="inlineStr"/>
       <c r="S97" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T97" t="inlineStr">
@@ -35392,7 +35392,7 @@
       <c r="R99" t="inlineStr"/>
       <c r="S99" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T99" t="inlineStr">
@@ -35536,7 +35536,7 @@
       <c r="R100" t="inlineStr"/>
       <c r="S100" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T100" t="inlineStr">
@@ -35680,7 +35680,7 @@
       <c r="R101" t="inlineStr"/>
       <c r="S101" t="inlineStr">
         <is>
-          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '65770fe25b3a1769d52dab53', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Actualización Home de Tienda', 'color': 'green_light', 'uses': 6}, {'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T101" t="inlineStr">
@@ -36127,7 +36127,7 @@
       <c r="R104" t="inlineStr"/>
       <c r="S104" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T104" t="inlineStr">
@@ -36972,7 +36972,7 @@
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T110" t="inlineStr">
@@ -37567,7 +37567,7 @@
       <c r="R114" t="inlineStr"/>
       <c r="S114" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T114" t="inlineStr">
@@ -37732,7 +37732,7 @@
       <c r="R115" t="inlineStr"/>
       <c r="S115" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T115" t="inlineStr">
@@ -38156,7 +38156,7 @@
       <c r="R118" t="inlineStr"/>
       <c r="S118" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T118" t="inlineStr">
@@ -38300,7 +38300,7 @@
       <c r="R119" t="inlineStr"/>
       <c r="S119" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T119" t="inlineStr">
@@ -38444,7 +38444,7 @@
       <c r="R120" t="inlineStr"/>
       <c r="S120" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T120" t="inlineStr">
@@ -38706,7 +38706,7 @@
       </c>
       <c r="S122" t="inlineStr">
         <is>
-          <t>[{'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}]</t>
+          <t>[{'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}, {'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}]</t>
         </is>
       </c>
       <c r="T122" t="inlineStr">
@@ -38832,7 +38832,7 @@
       </c>
       <c r="S123" t="inlineStr">
         <is>
-          <t>[{'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}]</t>
+          <t>[{'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}, {'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}]</t>
         </is>
       </c>
       <c r="T123" t="inlineStr">
@@ -38960,7 +38960,7 @@
       </c>
       <c r="S124" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}, {'id': '636bae21dec2010132392a0e', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Frontend', 'color': 'purple_dark', 'uses': 238}]</t>
         </is>
       </c>
       <c r="T124" t="inlineStr">
@@ -39115,7 +39115,7 @@
       <c r="R125" t="inlineStr"/>
       <c r="S125" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34df1', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Historia de Usuario', 'color': 'blue_dark', 'uses': 376}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T125" t="inlineStr">
@@ -39260,7 +39260,7 @@
       <c r="R126" t="inlineStr"/>
       <c r="S126" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}, {'id': '633e027dedd34201e1cc647c', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '📈 Data', 'color': 'purple_dark', 'uses': 104}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}, {'id': '633e027dedd34201e1cc647c', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '📈 Data', 'color': 'purple_dark', 'uses': 104}]</t>
         </is>
       </c>
       <c r="T126" t="inlineStr">
@@ -39408,7 +39408,7 @@
       <c r="R127" t="inlineStr"/>
       <c r="S127" t="inlineStr">
         <is>
-          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '6334975c28c9c402829c80e8', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '🦠️ Bug', 'color': 'red', 'uses': 322}, {'id': '649efb59907925786a331db5', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Producción', 'color': 'pink_dark', 'uses': 52}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T127" t="inlineStr">
@@ -39543,7 +39543,7 @@
       </c>
       <c r="S128" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 200}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfa', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Task', 'color': 'sky', 'uses': 384}, {'id': '63593e38b53cb103981ac979', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': '⚙️ BFF', 'color': 'yellow_light', 'uses': 199}]</t>
         </is>
       </c>
       <c r="T128" t="inlineStr">
@@ -39939,7 +39939,7 @@
       <c r="R131" t="inlineStr"/>
       <c r="S131" t="inlineStr">
         <is>
-          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 87}]</t>
+          <t>[{'id': '632b5ec4ee1230008bd34dfd', 'idBoard': '632b5ec4ee1230008bd34d6d', 'name': 'Technical Debt', 'color': 'lime_light', 'uses': 88}]</t>
         </is>
       </c>
       <c r="T131" t="inlineStr">

</xml_diff>